<commit_message>
Add user authentication with jwt. add controller action Register, Login, RefreshToken and RevokeToken
</commit_message>
<xml_diff>
--- a/E-Learning Project.xlsx
+++ b/E-Learning Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chula\Projects\E-Learning-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87466B7B-B127-4121-849D-5C28A329D63E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB25A5C-F5D6-4CFB-BFDE-B8CB5E9DF2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2166" yWindow="2166" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2394" yWindow="90" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>To Do</t>
   </si>
@@ -42,13 +42,6 @@
     <t>Finished</t>
   </si>
   <si>
-    <t>Setup Server Project</t>
-  </si>
-  <si>
-    <t>Work with User module
-and authentication with JWT</t>
-  </si>
-  <si>
     <t>Working</t>
   </si>
   <si>
@@ -58,41 +51,65 @@
     <t>Use Git and Github</t>
   </si>
   <si>
-    <t>Use @nestjs/jwt @nestjs/passport passport passport-jwt</t>
-  </si>
-  <si>
-    <t>Use NestJS and PostgreSQL 
-@nestjs/typeorm typeorm pg
-Add Validators:
-class-validator class-transformer</t>
-  </si>
-  <si>
     <t>Setup Web Api project using .Net 5.0</t>
+  </si>
+  <si>
+    <t>Setup Configuration</t>
+  </si>
+  <si>
+    <t>Add SqlConnection to appSetting.json, Add IdentityDbContext, Setup Configuration at Startup.cs</t>
+  </si>
+  <si>
+    <t>Add Swashbuckle.AspNetCore.Swagger, Swashbuckle.AspNetCore.SwaggerGen, Swashbuckle.AspNetCore.SwaggerUI</t>
+  </si>
+  <si>
+    <t>Setup Swagger and configure</t>
+  </si>
+  <si>
+    <t>Setup xml Documentation</t>
+  </si>
+  <si>
+    <t>Add xml Documentation at properties -&gt; build of the project. Supress warning and errors if need</t>
+  </si>
+  <si>
+    <t>Setup Logging</t>
+  </si>
+  <si>
+    <t>add NLog.Extensions.Logging,
+add nlog.config file at root,
+add LoggerService and configure it at Startup.cs</t>
+  </si>
+  <si>
+    <t>Setup Cors Policy</t>
+  </si>
+  <si>
+    <t>Add Cors Policy to interact with API with frontend</t>
   </si>
   <si>
     <t>Install Microsoft.EntityFrameworkCore
 Install Microsoft.EntityFrameworkCore.Design
 Install Microsoft.EntityFrameworkCore.Tools
 Install Npgsql.EntityFrameworkCore.PostgreSql
+Install Npgsql
 Install Microsoft.AspNetCore.Identity.EntityFrameworkCore</t>
   </si>
   <si>
-    <t>Setup Configuration</t>
-  </si>
-  <si>
-    <t>Add SqlConnection to appSetting.json, Add IdentityDbContext, Setup Configuration at Startup.cs</t>
-  </si>
-  <si>
-    <t>Add Swashbuckle.AspNetCore.Swagger, Swashbuckle.AspNetCore.SwaggerGen, Swashbuckle.AspNetCore.SwaggerUI</t>
-  </si>
-  <si>
-    <t>Setup Swagger and configure</t>
-  </si>
-  <si>
-    <t>Setup xml Documentation</t>
-  </si>
-  <si>
-    <t>Add xml Documentation at properties of the project</t>
+    <t>Add AppUser&lt;int&gt; and RoleUser&lt;int&gt; classes and update DbContext to
+IdentityDbContext&lt;AppUser, AppRole, int&gt;</t>
+  </si>
+  <si>
+    <t>Setup Identity Schema and Migrate
+with EntityFrameworkCore</t>
+  </si>
+  <si>
+    <t>Configure Authentication and Identity
+and authentication with JWT</t>
+  </si>
+  <si>
+    <t>Seed the sample User Data, Create UserController,
+Add controller actions for Signup, Login, Refrsh Token and Revoke Token
+Generate JWT, Set key and Issuer at appSetting file,
+Install Microsoft.AspNetCore.Authentication.JwtBearer</t>
   </si>
 </sst>
 </file>
@@ -416,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -435,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -444,12 +461,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
@@ -458,10 +475,10 @@
     </row>
     <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
@@ -470,70 +487,86 @@
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -554,6 +587,18 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add Refresh Token and Confirm Email.
</commit_message>
<xml_diff>
--- a/E-Learning Project.xlsx
+++ b/E-Learning Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Chula\Projects\E-Learning-API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB25A5C-F5D6-4CFB-BFDE-B8CB5E9DF2EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ACDBA5C-2BE0-4608-8A77-44349440AA1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2394" yWindow="90" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>To Do</t>
   </si>
@@ -110,6 +110,19 @@
 Add controller actions for Signup, Login, Refrsh Token and Revoke Token
 Generate JWT, Set key and Issuer at appSetting file,
 Install Microsoft.AspNetCore.Authentication.JwtBearer</t>
+  </si>
+  <si>
+    <t>Microsoft.AspNetCore.Mvc.NewtonsoftJson</t>
+  </si>
+  <si>
+    <t>AutoMapper, AutoMapper.Extensions.Microsoft.DependencyInjection</t>
+  </si>
+  <si>
+    <t>Sign in Email confirmation</t>
+  </si>
+  <si>
+    <t>Add .SignIn.RequireConfirmedEmail = true; to services.AddIdentity,
+Install NETCore.MailKit, Configure MailKitOptions at Startup.cs file, Add Email setting in the appSettings.json file.</t>
   </si>
 </sst>
 </file>
@@ -435,14 +448,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="35.41796875" customWidth="1"/>
-    <col min="2" max="2" width="52.3125" customWidth="1"/>
+    <col min="2" max="2" width="57.3671875" customWidth="1"/>
     <col min="3" max="3" width="12.578125" customWidth="1"/>
     <col min="4" max="4" width="14.41796875" customWidth="1"/>
   </cols>
@@ -571,19 +584,27 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
     </row>

</xml_diff>